<commit_message>
finally figured our joining issue
</commit_message>
<xml_diff>
--- a/Data/RespoFiles/Nutrient_Samples_ID.xlsx
+++ b/Data/RespoFiles/Nutrient_Samples_ID.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahmerges/Desktop/Repositories/Moorea_SGDdilutionassay_Metabolism/Data/RespoFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC00CA3-14B2-8F4B-8432-F54D8C3A3F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB04496-0DB8-3B4B-97F5-CBA8C5E5C5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="500" windowWidth="27240" windowHeight="15380" xr2:uid="{0C357FA3-1238-D54F-855A-53CFEA49DB67}"/>
+    <workbookView xWindow="1100" yWindow="1140" windowWidth="27240" windowHeight="15380" xr2:uid="{0C357FA3-1238-D54F-855A-53CFEA49DB67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1845,10 +1845,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1867,9 +1866,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1907,7 +1906,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2013,7 +2012,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2155,7 +2154,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2165,8 +2164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{350CA9E1-AF60-2949-BA90-04AE3C690A9C}">
   <dimension ref="A1:D439"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A426" workbookViewId="0">
-      <selection activeCell="C437" sqref="C437:C439"/>
+    <sheetView tabSelected="1" topLeftCell="A318" workbookViewId="0">
+      <selection activeCell="B328" sqref="B328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6463,7 +6462,7 @@
       <c r="A390" t="s">
         <v>389</v>
       </c>
-      <c r="B390" s="2" t="s">
+      <c r="B390" t="s">
         <v>571</v>
       </c>
       <c r="C390" s="1" t="s">
@@ -6562,7 +6561,7 @@
       <c r="A399" t="s">
         <v>398</v>
       </c>
-      <c r="B399" s="2" t="s">
+      <c r="B399" t="s">
         <v>571</v>
       </c>
       <c r="C399" s="1" t="s">
@@ -6661,7 +6660,7 @@
       <c r="A408" t="s">
         <v>407</v>
       </c>
-      <c r="B408" s="2" t="s">
+      <c r="B408" t="s">
         <v>571</v>
       </c>
       <c r="C408" s="1" t="s">
@@ -6760,7 +6759,7 @@
       <c r="A417" t="s">
         <v>416</v>
       </c>
-      <c r="B417" s="2" t="s">
+      <c r="B417" t="s">
         <v>571</v>
       </c>
       <c r="C417" s="1" t="s">
@@ -6859,7 +6858,7 @@
       <c r="A426" t="s">
         <v>425</v>
       </c>
-      <c r="B426" s="2" t="s">
+      <c r="B426" t="s">
         <v>571</v>
       </c>
       <c r="C426" s="1" t="s">
@@ -6958,7 +6957,7 @@
       <c r="A435" t="s">
         <v>434</v>
       </c>
-      <c r="B435" s="2" t="s">
+      <c r="B435" t="s">
         <v>571</v>
       </c>
       <c r="C435" s="1" t="s">

</xml_diff>